<commit_message>
Got full path working. Now to convert to macro form
</commit_message>
<xml_diff>
--- a/subpar_test/data/test_db.xlsx
+++ b/subpar_test/data/test_db.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Payments" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Payment" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -127,7 +127,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Can now parse two sheets. Cloning issues force redundancy, but fix it later
</commit_message>
<xml_diff>
--- a/subpar_test/data/test_db.xlsx
+++ b/subpar_test/data/test_db.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Payment" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Submission" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,15 +21,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">guid</t>
   </si>
   <si>
+    <t xml:space="preserve">PaYer</t>
+  </si>
+  <si>
     <t xml:space="preserve">F1-a</t>
   </si>
   <si>
+    <t xml:space="preserve">Odd</t>
+  </si>
+  <si>
     <t xml:space="preserve">F2-b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Even</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitting_org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEMC</t>
   </si>
 </sst>
 </file>
@@ -124,10 +143,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V23" activeCellId="0" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -139,15 +158,24 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -159,4 +187,57 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
It appears to work now. Time to integrate with the invoicer to see where the holes are
</commit_message>
<xml_diff>
--- a/subpar_test/data/test_db.xlsx
+++ b/subpar_test/data/test_db.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Payment" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Submission" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="payments" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="submissions" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -145,8 +145,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V23" activeCellId="0" sqref="V23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -196,8 +196,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V12" activeCellId="0" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>